<commit_message>
Extend BEB validation data
</commit_message>
<xml_diff>
--- a/data/tidy/BEB-validation.xlsx
+++ b/data/tidy/BEB-validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahsa\NARS\pv-trips-energy\data\tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690E0137-CBA1-416B-92F9-4B236082CDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CDD75D-F978-47AA-93F0-79A1AEDE4C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D275"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
         <v>1421</v>
       </c>
       <c r="B73">
-        <v>2010.7</v>
+        <v>201.7</v>
       </c>
       <c r="C73">
         <v>0.7</v>

</xml_diff>

<commit_message>
New space search for BEB model parameters
</commit_message>
<xml_diff>
--- a/data/tidy/BEB-validation.xlsx
+++ b/data/tidy/BEB-validation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahsa\NARS\pv-trips-energy\data\tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CDD75D-F978-47AA-93F0-79A1AEDE4C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E55E9C-471D-4A93-80B7-BE9507726FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$275</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -390,17 +393,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="39.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>3501</v>
       </c>
@@ -428,7 +431,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>3501</v>
       </c>
@@ -442,7 +445,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3501</v>
       </c>
@@ -456,7 +459,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>3501</v>
       </c>
@@ -470,7 +473,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>3501</v>
       </c>
@@ -484,7 +487,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>3501</v>
       </c>
@@ -498,7 +501,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>3501</v>
       </c>
@@ -512,7 +515,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>3501</v>
       </c>
@@ -526,7 +529,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>3501</v>
       </c>
@@ -540,7 +543,7 @@
         <v>44724</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>3501</v>
       </c>
@@ -554,7 +557,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>3501</v>
       </c>
@@ -568,7 +571,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>3501</v>
       </c>
@@ -582,7 +585,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>3501</v>
       </c>
@@ -596,7 +599,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>3501</v>
       </c>
@@ -610,7 +613,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>3501</v>
       </c>
@@ -624,7 +627,7 @@
         <v>44730</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>3501</v>
       </c>
@@ -638,7 +641,7 @@
         <v>44734</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>3501</v>
       </c>
@@ -652,7 +655,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>3501</v>
       </c>
@@ -666,7 +669,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>3501</v>
       </c>
@@ -680,7 +683,7 @@
         <v>44738</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>3501</v>
       </c>
@@ -694,7 +697,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>3501</v>
       </c>
@@ -708,7 +711,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>3501</v>
       </c>
@@ -722,7 +725,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>3501</v>
       </c>
@@ -736,7 +739,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>3501</v>
       </c>
@@ -750,7 +753,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>3501</v>
       </c>
@@ -764,7 +767,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>3501</v>
       </c>
@@ -778,7 +781,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>3501</v>
       </c>
@@ -792,7 +795,7 @@
         <v>44748</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>3501</v>
       </c>
@@ -806,7 +809,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>3501</v>
       </c>
@@ -820,7 +823,7 @@
         <v>44775</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>3501</v>
       </c>
@@ -834,7 +837,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>3501</v>
       </c>
@@ -848,7 +851,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>3501</v>
       </c>
@@ -862,7 +865,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>3501</v>
       </c>
@@ -876,7 +879,7 @@
         <v>44780</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>3501</v>
       </c>
@@ -890,7 +893,7 @@
         <v>44781</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>3501</v>
       </c>
@@ -904,7 +907,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>3501</v>
       </c>
@@ -918,7 +921,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>3501</v>
       </c>
@@ -932,7 +935,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>3501</v>
       </c>
@@ -946,7 +949,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>3501</v>
       </c>
@@ -960,7 +963,7 @@
         <v>44787</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>3501</v>
       </c>
@@ -974,7 +977,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>3501</v>
       </c>
@@ -988,7 +991,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>3501</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>3501</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>3501</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>3501</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>3501</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>3501</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>3501</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>3501</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>3501</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>3501</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>3501</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>3501</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>1323</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>44658</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>1323</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>44659</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A57">
         <v>1323</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A58">
         <v>1323</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A59">
         <v>1323</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>44663</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A60">
         <v>1323</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>44664</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A61">
         <v>1323</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A62">
         <v>1323</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>44666</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A63">
         <v>1323</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>44669</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A64">
         <v>1323</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A65">
         <v>1323</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A66">
         <v>1323</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>44676</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A67">
         <v>1323</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>44678</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A68">
         <v>1323</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>44679</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A69">
         <v>1323</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A70">
         <v>1421</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A71">
         <v>1421</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A72">
         <v>1421</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A73">
         <v>1421</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A74">
         <v>7700</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A75">
         <v>7700</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A76">
         <v>1421</v>
       </c>
@@ -1464,7 +1467,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A77">
         <v>1420</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A78">
         <v>1420</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>44790</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A79">
         <v>1420</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A80">
         <v>1420</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A81">
         <v>1420</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>44793</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A82">
         <v>1420</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A83">
         <v>1420</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A84">
         <v>1420</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A85">
         <v>1420</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A86">
         <v>1420</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A87">
         <v>1420</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A88">
         <v>1420</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A89">
         <v>1420</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A90">
         <v>1420</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A91">
         <v>1420</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A92">
         <v>1322</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A93">
         <v>1322</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>44775</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A94">
         <v>1322</v>
       </c>
@@ -1716,7 +1719,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A95">
         <v>1322</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A96">
         <v>1322</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A97">
         <v>1322</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>44779</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A98">
         <v>1322</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>44780</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A99">
         <v>1322</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>44781</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A100">
         <v>1322</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A101">
         <v>1322</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A102">
         <v>1322</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A103">
         <v>1322</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A104">
         <v>1322</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A105">
         <v>1322</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A106">
         <v>1322</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A107">
         <v>1322</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A108">
         <v>1322</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A109">
         <v>1421</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A110">
         <v>1421</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>44744</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A111">
         <v>1421</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A112">
         <v>1421</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>44746</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A113">
         <v>1421</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A114">
         <v>1421</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>44748</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A115">
         <v>7700</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A116">
         <v>1421</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A117">
         <v>1421</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>44751</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A118">
         <v>7700</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A119">
         <v>1421</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A120">
         <v>1421</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A121">
         <v>1421</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A122">
         <v>1421</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A123">
         <v>1421</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A124">
         <v>1421</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>44758</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A125">
         <v>1421</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>44760</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A126">
         <v>1421</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>44761</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A127">
         <v>1421</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>44762</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A128">
         <v>1421</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A129">
         <v>1421</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>44767</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A130">
         <v>1421</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>44768</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A131">
         <v>1421</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A132">
         <v>1421</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>44770</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A133">
         <v>7700</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>44771</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A134">
         <v>7700</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>44772</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A135">
         <v>7700</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A136">
         <v>1322</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A137">
         <v>1322</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A138">
         <v>1322</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A139">
         <v>1322</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A140">
         <v>1322</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>44751</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A141">
         <v>1322</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A142">
         <v>1322</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A143">
         <v>1322</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A144">
         <v>1322</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A145">
         <v>1322</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A146">
         <v>1322</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A147">
         <v>1322</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>44758</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A148">
         <v>1322</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>44760</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A149">
         <v>1322</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>44763</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A150">
         <v>1322</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A151">
         <v>1322</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>44765</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A152">
         <v>1322</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>44766</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A153">
         <v>1322</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>44767</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A154">
         <v>1322</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>44768</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A155">
         <v>1322</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>44771</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A156">
         <v>1421</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A157">
         <v>1421</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A158">
         <v>1421</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A159">
         <v>1421</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A160">
         <v>1421</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A161">
         <v>1421</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A162">
         <v>1421</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A163">
         <v>1421</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A164">
         <v>1421</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A165">
         <v>1421</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A166">
         <v>1421</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A167">
         <v>1421</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A168">
         <v>1421</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A169">
         <v>1421</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>44730</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A170">
         <v>1421</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>44731</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A171">
         <v>1421</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>44732</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A172">
         <v>1421</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>44733</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A173">
         <v>1421</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>44734</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A174">
         <v>1421</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A175">
         <v>1421</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A176">
         <v>1421</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A177">
         <v>1421</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A178">
         <v>1421</v>
       </c>
@@ -2892,7 +2895,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A179">
         <v>1421</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A180">
         <v>1421</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A181">
         <v>1321</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A182">
         <v>1321</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A183">
         <v>1321</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A184">
         <v>1321</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>44716</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A185">
         <v>1321</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A186">
         <v>1321</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A187">
         <v>1321</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A188">
         <v>1321</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A189">
         <v>1321</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A190">
         <v>1321</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A191">
         <v>1321</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A192">
         <v>1321</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A193">
         <v>1321</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A194">
         <v>1321</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A195">
         <v>1321</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>44732</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A196">
         <v>1321</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>44733</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A197">
         <v>1321</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A198">
         <v>1321</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A199">
         <v>1321</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A200">
         <v>1321</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>44738</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A201">
         <v>1321</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A202">
         <v>1321</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A203">
         <v>1321</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A204">
         <v>1323</v>
       </c>
@@ -3256,7 +3259,7 @@
         <v>44683</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A205">
         <v>1323</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A206">
         <v>1322</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A207">
         <v>1321</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>44686</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A208">
         <v>1321</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A209">
         <v>1321</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A210">
         <v>1321</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A211">
         <v>1321</v>
       </c>
@@ -3354,7 +3357,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A212">
         <v>1321</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>44694</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A213">
         <v>1323</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A214">
         <v>1321</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>44698</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A215">
         <v>1321</v>
       </c>
@@ -3410,7 +3413,7 @@
         <v>44699</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A216">
         <v>1321</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A217">
         <v>1321</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A218">
         <v>1321</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A219">
         <v>1321</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A220">
         <v>1321</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>44707</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A221">
         <v>1321</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>44708</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A222">
         <v>1321</v>
       </c>
@@ -3508,7 +3511,7 @@
         <v>44709</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A223">
         <v>1321</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A224">
         <v>1420</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A225">
         <v>1420</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>44806</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A226">
         <v>1420</v>
       </c>
@@ -3564,7 +3567,7 @@
         <v>44807</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A227">
         <v>1420</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A228">
         <v>1420</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A229">
         <v>1420</v>
       </c>
@@ -3606,7 +3609,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A230">
         <v>1420</v>
       </c>
@@ -3620,7 +3623,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A231">
         <v>1420</v>
       </c>
@@ -3634,7 +3637,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A232">
         <v>1420</v>
       </c>
@@ -3648,7 +3651,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A233">
         <v>1420</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A234">
         <v>1420</v>
       </c>
@@ -3676,7 +3679,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A235">
         <v>1420</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A236">
         <v>1420</v>
       </c>
@@ -3704,7 +3707,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A237">
         <v>1420</v>
       </c>
@@ -3718,7 +3721,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A238">
         <v>1420</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>44823</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A239">
         <v>1420</v>
       </c>
@@ -3746,7 +3749,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A240">
         <v>1420</v>
       </c>
@@ -3760,7 +3763,7 @@
         <v>44825</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A241">
         <v>1420</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A242">
         <v>1420</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A243">
         <v>7700</v>
       </c>
@@ -3802,7 +3805,7 @@
         <v>44828</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A244">
         <v>7700</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A245">
         <v>1420</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>44830</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A246">
         <v>1420</v>
       </c>
@@ -3844,12 +3847,12 @@
         <v>44831</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A247">
         <v>1420</v>
       </c>
       <c r="B247">
-        <v>37.6</v>
+        <v>255.8</v>
       </c>
       <c r="C247">
         <v>255.8</v>
@@ -3858,7 +3861,7 @@
         <v>44832</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A248">
         <v>1420</v>
       </c>
@@ -3872,7 +3875,7 @@
         <v>44833</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A249">
         <v>1420</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>44834</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A250">
         <v>1321</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A251">
         <v>1321</v>
       </c>
@@ -3914,7 +3917,7 @@
         <v>44806</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A252">
         <v>1321</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A253">
         <v>1321</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A254">
         <v>1321</v>
       </c>
@@ -3956,7 +3959,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A255">
         <v>1321</v>
       </c>
@@ -3970,7 +3973,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A256">
         <v>1323</v>
       </c>
@@ -3984,7 +3987,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A257">
         <v>1323</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A258">
         <v>1321</v>
       </c>
@@ -4012,7 +4015,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A259">
         <v>1321</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A260">
         <v>1321</v>
       </c>
@@ -4040,7 +4043,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A261">
         <v>1321</v>
       </c>
@@ -4054,7 +4057,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A262">
         <v>1321</v>
       </c>
@@ -4068,7 +4071,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A263">
         <v>1322</v>
       </c>
@@ -4082,7 +4085,7 @@
         <v>44821</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A264">
         <v>1323</v>
       </c>
@@ -4096,7 +4099,7 @@
         <v>44822</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A265">
         <v>1321</v>
       </c>
@@ -4110,7 +4113,7 @@
         <v>44823</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A266">
         <v>1321</v>
       </c>
@@ -4124,7 +4127,7 @@
         <v>44825</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A267">
         <v>1321</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A268">
         <v>1321</v>
       </c>
@@ -4152,7 +4155,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A269">
         <v>1321</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>44828</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A270">
         <v>1321</v>
       </c>
@@ -4180,7 +4183,7 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A271">
         <v>1321</v>
       </c>
@@ -4194,7 +4197,7 @@
         <v>44830</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A272">
         <v>1321</v>
       </c>
@@ -4208,7 +4211,7 @@
         <v>44831</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A273">
         <v>1321</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>44832</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A274">
         <v>1321</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>44833</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A275">
         <v>1321</v>
       </c>
@@ -4251,6 +4254,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D275" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calibration code for HEB and BEB
</commit_message>
<xml_diff>
--- a/data/tidy/BEB-validation.xlsx
+++ b/data/tidy/BEB-validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahsa\NARS\pv-trips-energy\data\tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E55E9C-471D-4A93-80B7-BE9507726FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB2DCD-CE24-41CA-9D85-7CFC32DF325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,19 +391,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B273" sqref="B273"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="4" max="4" width="39.1328125" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3501</v>
       </c>
@@ -431,7 +432,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3501</v>
       </c>
@@ -445,7 +446,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3501</v>
       </c>
@@ -459,7 +460,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3501</v>
       </c>
@@ -473,7 +474,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3501</v>
       </c>
@@ -487,7 +488,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3501</v>
       </c>
@@ -501,7 +502,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3501</v>
       </c>
@@ -515,7 +516,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3501</v>
       </c>
@@ -529,7 +530,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3501</v>
       </c>
@@ -543,7 +544,7 @@
         <v>44724</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3501</v>
       </c>
@@ -557,7 +558,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3501</v>
       </c>
@@ -571,7 +572,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3501</v>
       </c>
@@ -585,7 +586,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3501</v>
       </c>
@@ -599,7 +600,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3501</v>
       </c>
@@ -613,7 +614,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3501</v>
       </c>
@@ -627,7 +628,7 @@
         <v>44730</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3501</v>
       </c>
@@ -641,7 +642,7 @@
         <v>44734</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3501</v>
       </c>
@@ -655,7 +656,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3501</v>
       </c>
@@ -669,7 +670,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3501</v>
       </c>
@@ -683,7 +684,7 @@
         <v>44738</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3501</v>
       </c>
@@ -697,7 +698,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3501</v>
       </c>
@@ -711,7 +712,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3501</v>
       </c>
@@ -725,7 +726,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3501</v>
       </c>
@@ -739,7 +740,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3501</v>
       </c>
@@ -753,7 +754,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3501</v>
       </c>
@@ -767,7 +768,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3501</v>
       </c>
@@ -781,7 +782,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3501</v>
       </c>
@@ -795,7 +796,7 @@
         <v>44748</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3501</v>
       </c>
@@ -809,7 +810,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3501</v>
       </c>
@@ -823,7 +824,7 @@
         <v>44775</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3501</v>
       </c>
@@ -837,7 +838,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3501</v>
       </c>
@@ -851,7 +852,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3501</v>
       </c>
@@ -865,7 +866,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3501</v>
       </c>
@@ -879,7 +880,7 @@
         <v>44780</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3501</v>
       </c>
@@ -893,7 +894,7 @@
         <v>44781</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3501</v>
       </c>
@@ -907,7 +908,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3501</v>
       </c>
@@ -921,7 +922,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3501</v>
       </c>
@@ -935,7 +936,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3501</v>
       </c>
@@ -949,7 +950,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3501</v>
       </c>
@@ -963,7 +964,7 @@
         <v>44787</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3501</v>
       </c>
@@ -977,7 +978,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3501</v>
       </c>
@@ -991,7 +992,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3501</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3501</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3501</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3501</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3501</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3501</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3501</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3501</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3501</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3501</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3501</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3501</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1323</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>44658</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1323</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>44659</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1323</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1323</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1323</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>44663</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1323</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>44664</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1323</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1323</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>44666</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1323</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>44669</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1323</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1323</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1323</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>44676</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1323</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>44678</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1323</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>44679</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1323</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1421</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1421</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1421</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1421</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7700</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>7700</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1421</v>
       </c>
@@ -1467,7 +1468,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1420</v>
       </c>
@@ -1481,7 +1482,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1420</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>44790</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1420</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1420</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1420</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>44793</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1420</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1420</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1420</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1420</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1420</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1420</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1420</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1420</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1420</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1420</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1322</v>
       </c>
@@ -1691,7 +1692,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1322</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>44775</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1322</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1322</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1322</v>
       </c>
@@ -1747,7 +1748,7 @@
         <v>44778</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1322</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>44779</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1322</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>44780</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1322</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>44781</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1322</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>44782</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1322</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1322</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1322</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>44785</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1322</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1322</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>44789</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1322</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1322</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1322</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1421</v>
       </c>
@@ -1929,7 +1930,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1421</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>44744</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1421</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1421</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>44746</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1421</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1421</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>44748</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>7700</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1421</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1421</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>44751</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>7700</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1421</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1421</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1421</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1421</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1421</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1421</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>44758</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1421</v>
       </c>
@@ -2153,7 +2154,7 @@
         <v>44760</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1421</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>44761</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1421</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>44762</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1421</v>
       </c>
@@ -2195,7 +2196,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1421</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>44767</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1421</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>44768</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>1421</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1421</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>44770</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>7700</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>44771</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>7700</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>44772</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7700</v>
       </c>
@@ -2293,7 +2294,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1322</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1322</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1322</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1322</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1322</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>44751</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1322</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1322</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1322</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1322</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1322</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1322</v>
       </c>
@@ -2447,7 +2448,7 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1322</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>44758</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1322</v>
       </c>
@@ -2475,7 +2476,7 @@
         <v>44760</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1322</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>44763</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1322</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1322</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>44765</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1322</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>44766</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1322</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>44767</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1322</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>44768</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1322</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>44771</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1421</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1421</v>
       </c>
@@ -2601,7 +2602,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1421</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1421</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1421</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1421</v>
       </c>
@@ -2657,7 +2658,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1421</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1421</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1421</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1421</v>
       </c>
@@ -2713,7 +2714,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1421</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1421</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1421</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1421</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>44730</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1421</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>44731</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1421</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>44732</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1421</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>44733</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1421</v>
       </c>
@@ -2825,7 +2826,7 @@
         <v>44734</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1421</v>
       </c>
@@ -2839,7 +2840,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1421</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1421</v>
       </c>
@@ -2867,7 +2868,7 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1421</v>
       </c>
@@ -2881,7 +2882,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1421</v>
       </c>
@@ -2895,7 +2896,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1421</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1421</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1321</v>
       </c>
@@ -2937,7 +2938,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1321</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1321</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1321</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>44716</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1321</v>
       </c>
@@ -2993,7 +2994,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1321</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>1321</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>44720</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1321</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>44721</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1321</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1321</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>44725</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1321</v>
       </c>
@@ -3077,7 +3078,7 @@
         <v>44726</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1321</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1321</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>44728</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1321</v>
       </c>
@@ -3119,7 +3120,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1321</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>44732</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1321</v>
       </c>
@@ -3147,7 +3148,7 @@
         <v>44733</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>1321</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>1321</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>1321</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>1321</v>
       </c>
@@ -3203,7 +3204,7 @@
         <v>44738</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1321</v>
       </c>
@@ -3217,7 +3218,7 @@
         <v>44739</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>1321</v>
       </c>
@@ -3231,7 +3232,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1321</v>
       </c>
@@ -3245,7 +3246,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>1323</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>44683</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>1323</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>1322</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1321</v>
       </c>
@@ -3301,7 +3302,7 @@
         <v>44686</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1321</v>
       </c>
@@ -3315,7 +3316,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1321</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1321</v>
       </c>
@@ -3343,7 +3344,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1321</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1321</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>44694</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1323</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1321</v>
       </c>
@@ -3399,7 +3400,7 @@
         <v>44698</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1321</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>44699</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1321</v>
       </c>
@@ -3427,7 +3428,7 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1321</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1321</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>1321</v>
       </c>
@@ -3469,7 +3470,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1321</v>
       </c>
@@ -3483,7 +3484,7 @@
         <v>44707</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>1321</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>44708</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>1321</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>44709</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1321</v>
       </c>
@@ -3525,7 +3526,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>1420</v>
       </c>
@@ -3539,7 +3540,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>1420</v>
       </c>
@@ -3553,7 +3554,7 @@
         <v>44806</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1420</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>44807</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>1420</v>
       </c>
@@ -3581,7 +3582,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1420</v>
       </c>
@@ -3595,7 +3596,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>1420</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>1420</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1420</v>
       </c>
@@ -3637,7 +3638,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>1420</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1420</v>
       </c>
@@ -3665,7 +3666,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>1420</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>1420</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>1420</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>1420</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1420</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>44823</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>1420</v>
       </c>
@@ -3749,7 +3750,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>1420</v>
       </c>
@@ -3763,7 +3764,7 @@
         <v>44825</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>1420</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>1420</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>7700</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>44828</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>7700</v>
       </c>
@@ -3819,7 +3820,7 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>1420</v>
       </c>
@@ -3833,7 +3834,7 @@
         <v>44830</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1420</v>
       </c>
@@ -3847,12 +3848,12 @@
         <v>44831</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1420</v>
       </c>
       <c r="B247">
-        <v>255.8</v>
+        <v>37.6</v>
       </c>
       <c r="C247">
         <v>255.8</v>
@@ -3861,7 +3862,7 @@
         <v>44832</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1420</v>
       </c>
@@ -3875,7 +3876,7 @@
         <v>44833</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1420</v>
       </c>
@@ -3889,7 +3890,7 @@
         <v>44834</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1321</v>
       </c>
@@ -3903,7 +3904,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1321</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>44806</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1321</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1321</v>
       </c>
@@ -3945,7 +3946,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1321</v>
       </c>
@@ -3959,7 +3960,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>1321</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1323</v>
       </c>
@@ -3987,7 +3988,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1323</v>
       </c>
@@ -4001,7 +4002,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1321</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>1321</v>
       </c>
@@ -4029,7 +4030,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>1321</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>1321</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>1321</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1322</v>
       </c>
@@ -4085,7 +4086,7 @@
         <v>44821</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1323</v>
       </c>
@@ -4099,7 +4100,7 @@
         <v>44822</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>1321</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>44823</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1321</v>
       </c>
@@ -4127,7 +4128,7 @@
         <v>44825</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>1321</v>
       </c>
@@ -4141,7 +4142,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1321</v>
       </c>
@@ -4155,7 +4156,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>1321</v>
       </c>
@@ -4169,7 +4170,7 @@
         <v>44828</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1321</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1321</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>44830</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1321</v>
       </c>
@@ -4211,7 +4212,7 @@
         <v>44831</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1321</v>
       </c>
@@ -4225,7 +4226,7 @@
         <v>44832</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1321</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>44833</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>1321</v>
       </c>
@@ -4254,7 +4255,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D275" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D275" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <dateGroupItem year="2022" month="9" day="28" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>